<commit_message>
level logger well 2019 data
</commit_message>
<xml_diff>
--- a/WL_Well/Locations/Solinst_SerialNumber_2022.xlsx
+++ b/WL_Well/Locations/Solinst_SerialNumber_2022.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kriddie\OneDrive - University of North Carolina at Chapel Hill\Documents\LongTermData_CayambeCoca\LongTerm_WellData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kriddie\OneDrive - University of North Carolina at Chapel Hill\Documents\LongTermData_CayambeCoca\WL_Well\Locations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EE32BA-7002-496F-BE00-0D037184C5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B964F2F5-F1C4-4A31-8C92-CC6A210622F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41865" yWindow="900" windowWidth="18990" windowHeight="15150" xr2:uid="{51E9588E-32B4-C74E-BFD3-897853E1E191}"/>
+    <workbookView xWindow="30105" yWindow="0" windowWidth="18990" windowHeight="15150" xr2:uid="{51E9588E-32B4-C74E-BFD3-897853E1E191}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Location</t>
   </si>
   <si>
-    <t>serial number</t>
-  </si>
-  <si>
     <t>Gavilan</t>
   </si>
   <si>
@@ -65,16 +63,16 @@
     <t>Across from Lake</t>
   </si>
   <si>
-    <t>Lower</t>
-  </si>
-  <si>
     <t>Parqueadero</t>
   </si>
   <si>
     <t xml:space="preserve">center </t>
   </si>
   <si>
-    <t>** middle of wetland areaish</t>
+    <t>serial number 2022</t>
+  </si>
+  <si>
+    <t>Lower ( middle of wetland areaish)</t>
   </si>
 </sst>
 </file>
@@ -447,7 +445,7 @@
   <dimension ref="A4:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -462,15 +460,15 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -481,10 +479,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
       </c>
       <c r="C6">
         <v>2106253</v>
@@ -492,57 +490,63 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>2020442</v>
       </c>
+      <c r="D7">
+        <v>72020442</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
       </c>
       <c r="C8">
         <v>2020437</v>
       </c>
+      <c r="D8">
+        <v>72020437</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>2020435</v>
       </c>
+      <c r="D9">
+        <v>78020435</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>2020431</v>
       </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>2020433</v>

</xml_diff>